<commit_message>
- evaluation of multiple expressions separated by comma
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/TryToLoad/PrintArea.xlsx
+++ b/ClosedXML_Tests/Resource/TryToLoad/PrintArea.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X60019379\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DocumentPartner.ClosedXML\ClosedXML_Tests\Resource\TryToLoad\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBB52E0-1F86-4993-A4C8-11E22F1C3882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16890" windowHeight="3060"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Rohdaten" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Tabelle 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Rohdaten" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">IF(Rohdaten!$A$2&lt;5,Tabelle1!$A$1:$C$40,Tabelle1!$A$1:$C$80)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">IF(Rohdaten!$A$2&lt;5,'Tabelle 1'!$A$1:$C$40,'Tabelle 1'!$A$1:$C$80)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">IF(Rohdaten!$A$2&lt;5,'Tabelle 2'!$A$1:$C$40,'Tabelle 2'!$A$1:$C$80),'Tabelle 2'!$J$17:$M$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Tabelle 3'!$C$4:$G$12,'Tabelle 3'!$F$17:$J$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,7 +74,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,14 +351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -374,14 +379,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC706DC-B664-4E11-85F2-884BA027190D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD0BE5E-A0F5-4B93-B5B1-24AA1329CBCA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- using LastIndexOf in order to handle sheetNames with exclamation mark
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/TryToLoad/PrintArea.xlsx
+++ b/ClosedXML_Tests/Resource/TryToLoad/PrintArea.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DocumentPartner.ClosedXML\ClosedXML_Tests\Resource\TryToLoad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBB52E0-1F86-4993-A4C8-11E22F1C3882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B6444-9E69-4AE4-89D5-56ACD7A66C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle 2" sheetId="3" r:id="rId2"/>
     <sheet name="Tabelle 3" sheetId="4" r:id="rId3"/>
-    <sheet name="Rohdaten" sheetId="2" r:id="rId4"/>
+    <sheet name="Rohdaten !" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">IF(Rohdaten!$A$2&lt;5,'Tabelle 1'!$A$1:$C$40,'Tabelle 1'!$A$1:$C$80)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">IF(Rohdaten!$A$2&lt;5,'Tabelle 2'!$A$1:$C$40,'Tabelle 2'!$A$1:$C$80),'Tabelle 2'!$J$17:$M$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">IF('Rohdaten !'!$A$2&lt;5,'Tabelle 1'!$A$1:$C$40,'Tabelle 1'!$A$1:$C$80)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">IF('Rohdaten !'!$A$2&lt;5,'Tabelle 2'!$A$1:$C$40,'Tabelle 2'!$A$1:$C$80),'Tabelle 2'!$J$17:$M$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Tabelle 3'!$C$4:$G$12,'Tabelle 3'!$F$17:$J$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -356,9 +356,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -382,11 +382,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC706DC-B664-4E11-85F2-884BA027190D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -410,11 +410,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- also handling defined names for print areas
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/TryToLoad/PrintArea.xlsx
+++ b/ClosedXML_Tests/Resource/TryToLoad/PrintArea.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DocumentPartner.ClosedXML\ClosedXML_Tests\Resource\TryToLoad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B6444-9E69-4AE4-89D5-56ACD7A66C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8402F6-BAA5-4250-AABD-300E954F5736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle 1" sheetId="1" r:id="rId1"/>

</xml_diff>